<commit_message>
Update NGS analysis stats
</commit_message>
<xml_diff>
--- a/B.Scripts_and_bioinformatic_pipelines/B2.NGS_analysis/SRA_data.xlsx
+++ b/B.Scripts_and_bioinformatic_pipelines/B2.NGS_analysis/SRA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bea\Dropbox\BAR\CVB3_P1P2P3_dms\P1P2P3_manuscript\github\B.Scripts_and_bioinformatic_pipelines\B2.NGS_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron Geller\Dropbox\LAB\Lab_people\BAR\CVB3_P1P2P3_dms\P1P2P3_manuscript\Actual_github\CVB3_full_proteome_DMS\B.Scripts_and_bioinformatic_pipelines\B2.NGS_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD01CC4E-83BF-4D6B-9F8A-583A44F72674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91250051-7BE5-4111-8226-BB62466FF62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -427,9 +425,6 @@
     <t>C1_rP1_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P1 library 1 in RPE cells</t>
-  </si>
-  <si>
     <t>C1_rP1_RPE.bam</t>
   </si>
   <si>
@@ -442,9 +437,6 @@
     <t>C2_rP1_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P1 library 2 in RPE cells</t>
-  </si>
-  <si>
     <t>C2_rP1_RPE.bam</t>
   </si>
   <si>
@@ -457,9 +449,6 @@
     <t>C1_rP2_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 1 in RPE cells</t>
-  </si>
-  <si>
     <t>C1_rP2_RPE.bam</t>
   </si>
   <si>
@@ -472,9 +461,6 @@
     <t>C2_rP2_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 2 in RPE cells</t>
-  </si>
-  <si>
     <t>C2_rP2_RPE.bam</t>
   </si>
   <si>
@@ -487,9 +473,6 @@
     <t>C3_rP2_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 3 in RPE cells</t>
-  </si>
-  <si>
     <t>C3_rP2_RPE.bam</t>
   </si>
   <si>
@@ -502,9 +485,6 @@
     <t>C1_rP3_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 1 in RPE cells</t>
-  </si>
-  <si>
     <t>C1_rP3_RPE.bam</t>
   </si>
   <si>
@@ -517,9 +497,6 @@
     <t>C2_rP3_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 2 in RPE cells</t>
-  </si>
-  <si>
     <t>C2_rP3_RPE.bam</t>
   </si>
   <si>
@@ -532,9 +509,6 @@
     <t>C3_rP3_RPE</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 3 in RPE cells</t>
-  </si>
-  <si>
     <t>C3_rP3_RPE.bam</t>
   </si>
   <si>
@@ -583,9 +557,6 @@
     <t>C1_rP2_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 1</t>
-  </si>
-  <si>
     <t>C1_rP2_HeLa.bam</t>
   </si>
   <si>
@@ -598,9 +569,6 @@
     <t>C2_rP2_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 2</t>
-  </si>
-  <si>
     <t>C2_rP2_HeLa.bam</t>
   </si>
   <si>
@@ -613,9 +581,6 @@
     <t>C3_rP2_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P2 library 3</t>
-  </si>
-  <si>
     <t>C3_rP2_HeLa.bam</t>
   </si>
   <si>
@@ -628,9 +593,6 @@
     <t>C1_rP3_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 1</t>
-  </si>
-  <si>
     <t>C1_rP3_HeLa.bam</t>
   </si>
   <si>
@@ -643,9 +605,6 @@
     <t>C2_rP3_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 2</t>
-  </si>
-  <si>
     <t>C2_rP3_HeLa.bam</t>
   </si>
   <si>
@@ -658,9 +617,6 @@
     <t>C3_rP3_HeLa</t>
   </si>
   <si>
-    <t>CVB3 virus from passage 1 of the mutagenized P3 library 3</t>
-  </si>
-  <si>
     <t>C3_rP3_HeLa.bam</t>
   </si>
   <si>
@@ -764,6 +720,48 @@
   </si>
   <si>
     <t>new_adaptors (8N)</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 1</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 2</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 3</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 1</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 2</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 3</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P1 library 1 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P1 library 2 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 1 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 2 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P2 library 3 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 1 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 2 in RPE cells</t>
+  </si>
+  <si>
+    <t>CVB3 virus from passage 2 of the mutagenized P3 library 3 in RPE cells</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1091,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1118,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1177,12 +1175,12 @@
         <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1224,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="P2" t="s">
         <v>29</v>
@@ -1239,12 +1237,12 @@
         <v>35</v>
       </c>
       <c r="T2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -1286,7 +1284,7 @@
         <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="P3" t="s">
         <v>29</v>
@@ -1301,12 +1299,12 @@
         <v>41</v>
       </c>
       <c r="T3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
@@ -1348,7 +1346,7 @@
         <v>25</v>
       </c>
       <c r="O4" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="P4" t="s">
         <v>29</v>
@@ -1363,12 +1361,12 @@
         <v>49</v>
       </c>
       <c r="T4" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -1410,7 +1408,7 @@
         <v>25</v>
       </c>
       <c r="O5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="P5" t="s">
         <v>29</v>
@@ -1425,12 +1423,12 @@
         <v>54</v>
       </c>
       <c r="T5" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
@@ -1472,7 +1470,7 @@
         <v>25</v>
       </c>
       <c r="O6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="P6" t="s">
         <v>29</v>
@@ -1487,12 +1485,12 @@
         <v>59</v>
       </c>
       <c r="T6" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
@@ -1534,7 +1532,7 @@
         <v>25</v>
       </c>
       <c r="O7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P7" t="s">
         <v>29</v>
@@ -1549,12 +1547,12 @@
         <v>79</v>
       </c>
       <c r="T7" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
@@ -1596,7 +1594,7 @@
         <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="P8" t="s">
         <v>29</v>
@@ -1611,12 +1609,12 @@
         <v>64</v>
       </c>
       <c r="T8" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
         <v>65</v>
@@ -1658,7 +1656,7 @@
         <v>25</v>
       </c>
       <c r="O9" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="P9" t="s">
         <v>29</v>
@@ -1673,12 +1671,12 @@
         <v>69</v>
       </c>
       <c r="T9" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -1720,7 +1718,7 @@
         <v>25</v>
       </c>
       <c r="O10" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="P10" t="s">
         <v>29</v>
@@ -1735,12 +1733,12 @@
         <v>74</v>
       </c>
       <c r="T10" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
         <v>80</v>
@@ -1782,7 +1780,7 @@
         <v>25</v>
       </c>
       <c r="O11" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P11" t="s">
         <v>29</v>
@@ -1797,12 +1795,12 @@
         <v>84</v>
       </c>
       <c r="T11" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
         <v>87</v>
@@ -1844,7 +1842,7 @@
         <v>25</v>
       </c>
       <c r="O12" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="P12" t="s">
         <v>29</v>
@@ -1859,12 +1857,12 @@
         <v>91</v>
       </c>
       <c r="T12" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
         <v>92</v>
@@ -1906,7 +1904,7 @@
         <v>25</v>
       </c>
       <c r="O13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="P13" t="s">
         <v>29</v>
@@ -1921,12 +1919,12 @@
         <v>96</v>
       </c>
       <c r="T13" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
         <v>97</v>
@@ -1983,15 +1981,15 @@
         <v>101</v>
       </c>
       <c r="T14" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
         <v>117</v>
@@ -2003,16 +2001,16 @@
         <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H15" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I15" t="s">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="J15" t="s">
         <v>21</v>
@@ -2042,18 +2040,18 @@
         <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="T15" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
         <v>117</v>
@@ -2065,16 +2063,16 @@
         <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G16" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="I16" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="J16" t="s">
         <v>21</v>
@@ -2104,18 +2102,18 @@
         <v>28</v>
       </c>
       <c r="S16" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="T16" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
         <v>117</v>
@@ -2127,16 +2125,16 @@
         <v>118</v>
       </c>
       <c r="F17" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G17" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H17" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I17" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="J17" t="s">
         <v>21</v>
@@ -2166,15 +2164,15 @@
         <v>28</v>
       </c>
       <c r="S17" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="T17" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
         <v>102</v>
@@ -2231,12 +2229,12 @@
         <v>106</v>
       </c>
       <c r="T18" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
         <v>107</v>
@@ -2293,12 +2291,12 @@
         <v>111</v>
       </c>
       <c r="T19" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
         <v>112</v>
@@ -2355,15 +2353,15 @@
         <v>116</v>
       </c>
       <c r="T20" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
         <v>117</v>
@@ -2375,16 +2373,16 @@
         <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="I21" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
       <c r="J21" t="s">
         <v>21</v>
@@ -2414,18 +2412,18 @@
         <v>28</v>
       </c>
       <c r="S21" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="T21" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
         <v>117</v>
@@ -2437,16 +2435,16 @@
         <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="G22" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="H22" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="I22" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="J22" t="s">
         <v>21</v>
@@ -2476,18 +2474,18 @@
         <v>28</v>
       </c>
       <c r="S22" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="T22" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
         <v>117</v>
@@ -2499,16 +2497,16 @@
         <v>118</v>
       </c>
       <c r="F23" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G23" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="H23" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="I23" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="J23" t="s">
         <v>21</v>
@@ -2538,15 +2536,15 @@
         <v>28</v>
       </c>
       <c r="S23" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="T23" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
         <v>119</v>
@@ -2570,7 +2568,7 @@
         <v>121</v>
       </c>
       <c r="I24" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="J24" t="s">
         <v>21</v>
@@ -2600,18 +2598,18 @@
         <v>28</v>
       </c>
       <c r="S24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T24" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
         <v>117</v>
@@ -2623,16 +2621,16 @@
         <v>118</v>
       </c>
       <c r="F25" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" t="s">
         <v>125</v>
       </c>
-      <c r="G25" t="s">
-        <v>126</v>
-      </c>
       <c r="H25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I25" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="J25" t="s">
         <v>21</v>
@@ -2662,18 +2660,18 @@
         <v>28</v>
       </c>
       <c r="S25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T25" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
         <v>117</v>
@@ -2685,16 +2683,16 @@
         <v>118</v>
       </c>
       <c r="F26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I26" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
       <c r="J26" t="s">
         <v>21</v>
@@ -2724,18 +2722,18 @@
         <v>28</v>
       </c>
       <c r="S26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="T26" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
         <v>117</v>
@@ -2747,16 +2745,16 @@
         <v>118</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I27" t="s">
-        <v>137</v>
+        <v>230</v>
       </c>
       <c r="J27" t="s">
         <v>21</v>
@@ -2786,18 +2784,18 @@
         <v>28</v>
       </c>
       <c r="S27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="T27" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
         <v>117</v>
@@ -2809,16 +2807,16 @@
         <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I28" t="s">
-        <v>142</v>
+        <v>231</v>
       </c>
       <c r="J28" t="s">
         <v>21</v>
@@ -2848,18 +2846,18 @@
         <v>28</v>
       </c>
       <c r="S28" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="T28" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
         <v>117</v>
@@ -2871,16 +2869,16 @@
         <v>118</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G29" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H29" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="J29" t="s">
         <v>21</v>
@@ -2910,18 +2908,18 @@
         <v>28</v>
       </c>
       <c r="S29" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="T29" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
         <v>117</v>
@@ -2933,16 +2931,16 @@
         <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G30" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H30" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="I30" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="J30" t="s">
         <v>21</v>
@@ -2972,18 +2970,18 @@
         <v>28</v>
       </c>
       <c r="S30" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="T30" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
         <v>117</v>
@@ -2995,16 +2993,16 @@
         <v>118</v>
       </c>
       <c r="F31" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I31" t="s">
-        <v>157</v>
+        <v>234</v>
       </c>
       <c r="J31" t="s">
         <v>21</v>
@@ -3034,10 +3032,10 @@
         <v>28</v>
       </c>
       <c r="S31" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="T31" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>